<commit_message>
Update 3-) Turkiye'de tekstil ithalat ve ihracat hacmi.xlsx
</commit_message>
<xml_diff>
--- a/3-) Turkiye'de tekstil ithalat ve ihracat hacmi.xlsx
+++ b/3-) Turkiye'de tekstil ithalat ve ihracat hacmi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fintegral365-my.sharepoint.com/personal/oguz_oztekin_fintegral_com_tr/Documents/Masaüstü/Dis-Ticaret-Tekstil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3CBF4731BA31921FD2FE31D2F8F2D3C2245755F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B352D333-C3F6-4FCF-BA8F-BCA1F0B1B9AD}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_868981054830921FD2FE31D2F8F2D3C2145669F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53F217CA-03EF-445E-959F-C0A3AA477038}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Yıl</t>
   </si>
   <si>
-    <t>Türkiyenin Toplam Ticaret Hacmi</t>
+    <t>Türkiyenin Toplam İhracat Hacmi</t>
   </si>
   <si>
     <t>Tekstil İhracat Hacmi</t>
+  </si>
+  <si>
+    <t>Türkiyenin Toplam İthalat Hacmi</t>
   </si>
   <si>
     <t>Tekstil İthalat Hacmi</t>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,12 +419,13 @@
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,205 +444,238 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2012</v>
       </c>
       <c r="B2">
-        <v>370432661.03799999</v>
+        <v>160179713.31900001</v>
       </c>
       <c r="C2">
         <v>30095689.348999999</v>
       </c>
       <c r="D2">
+        <v>210252947.71900001</v>
+      </c>
+      <c r="E2">
         <v>13962093.619999999</v>
       </c>
-      <c r="E2">
-        <v>8.1244697118952747</v>
-      </c>
       <c r="F2">
-        <v>3.769131366785103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18.78870221790449</v>
+      </c>
+      <c r="G2">
+        <v>6.6406173000057684</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2013</v>
       </c>
       <c r="B3">
-        <v>404765658.36000001</v>
+        <v>169897259.215</v>
       </c>
       <c r="C3">
         <v>33531121.298999999</v>
       </c>
       <c r="D3">
+        <v>234868399.14500001</v>
+      </c>
+      <c r="E3">
         <v>15808607.267000001</v>
       </c>
-      <c r="E3">
-        <v>8.2840825565239271</v>
-      </c>
       <c r="F3">
-        <v>3.9056196938871151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19.736116670703531</v>
+      </c>
+      <c r="G3">
+        <v>6.7308362148967884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2014</v>
       </c>
       <c r="B4">
-        <v>404860279.40100002</v>
+        <v>176114435.222</v>
       </c>
       <c r="C4">
         <v>35381391.788999997</v>
       </c>
       <c r="D4">
+        <v>228745844.17899999</v>
+      </c>
+      <c r="E4">
         <v>16623453.663000001</v>
       </c>
-      <c r="E4">
-        <v>8.7391610363327246</v>
-      </c>
       <c r="F4">
-        <v>4.1059729760585002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20.09000099531886</v>
+      </c>
+      <c r="G4">
+        <v>7.2672155958346876</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2015</v>
       </c>
       <c r="B5">
-        <v>361425100.16100001</v>
+        <v>161303390.877</v>
       </c>
       <c r="C5">
         <v>32209204.732000001</v>
       </c>
       <c r="D5">
+        <v>200121709.28400001</v>
+      </c>
+      <c r="E5">
         <v>14066801.130999999</v>
       </c>
-      <c r="E5">
-        <v>8.9117232637279837</v>
-      </c>
       <c r="F5">
-        <v>3.8920376932132879</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19.968089050626809</v>
+      </c>
+      <c r="G5">
+        <v>7.0291230178517461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2016</v>
       </c>
       <c r="B6">
-        <v>358511912.54400003</v>
+        <v>162033589.39500001</v>
       </c>
       <c r="C6">
         <v>32288441</v>
       </c>
       <c r="D6">
+        <v>196478323.14899999</v>
+      </c>
+      <c r="E6">
         <v>13576427.028000001</v>
       </c>
-      <c r="E6">
-        <v>9.0062393661848699</v>
-      </c>
       <c r="F6">
-        <v>3.7868831001072438</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19.927004715848351</v>
+      </c>
+      <c r="G6">
+        <v>6.9098854318418983</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2017</v>
       </c>
       <c r="B7">
-        <v>392797816.92699999</v>
+        <v>170238045.59599999</v>
       </c>
       <c r="C7">
         <v>32096123.363000002</v>
       </c>
       <c r="D7">
+        <v>222559771.331</v>
+      </c>
+      <c r="E7">
         <v>14146714.736</v>
       </c>
-      <c r="E7">
-        <v>8.1711562488049534</v>
-      </c>
       <c r="F7">
-        <v>3.6015258044647211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18.85367236837812</v>
+      </c>
+      <c r="G7">
+        <v>6.3563664948956244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
       <c r="B8">
-        <v>398575871.12599999</v>
+        <v>188343441.39899999</v>
       </c>
       <c r="C8">
         <v>34356543.740999997</v>
       </c>
       <c r="D8">
+        <v>210232429.727</v>
+      </c>
+      <c r="E8">
         <v>13154557.202</v>
       </c>
-      <c r="E8">
-        <v>8.6198252904624582</v>
-      </c>
       <c r="F8">
-        <v>3.3003897513508811</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18.24143356721229</v>
+      </c>
+      <c r="G8">
+        <v>6.2571493936886986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2019</v>
       </c>
       <c r="B9">
-        <v>385052427.81999999</v>
+        <v>190669538.46900001</v>
       </c>
       <c r="C9">
         <v>35163473.479000002</v>
       </c>
       <c r="D9">
+        <v>194382889.35100001</v>
+      </c>
+      <c r="E9">
         <v>12596212.357000001</v>
       </c>
-      <c r="E9">
-        <v>9.1321261569704539</v>
-      </c>
       <c r="F9">
-        <v>3.271297996564857</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18.442103422155739</v>
+      </c>
+      <c r="G9">
+        <v>6.4801034695264947</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2020</v>
       </c>
       <c r="B10">
-        <v>388456798.85699999</v>
+        <v>179376774.61500001</v>
       </c>
       <c r="C10">
         <v>33316839.557</v>
       </c>
       <c r="D10">
+        <v>209080024.24200001</v>
+      </c>
+      <c r="E10">
         <v>10752021.278000001</v>
       </c>
-      <c r="E10">
-        <v>8.5767168073855</v>
-      </c>
       <c r="F10">
-        <v>2.7678808324727169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18.57366408137765</v>
+      </c>
+      <c r="G10">
+        <v>5.1425387561439422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2021</v>
       </c>
       <c r="B11">
-        <v>481522501.03899997</v>
+        <v>233216566.11500001</v>
       </c>
       <c r="C11">
         <v>41736981.439999998</v>
       </c>
       <c r="D11">
+        <v>248305934.92399999</v>
+      </c>
+      <c r="E11">
         <v>13635222.971000001</v>
       </c>
-      <c r="E11">
-        <v>8.6677115503309761</v>
-      </c>
       <c r="F11">
-        <v>2.8316896804570391</v>
+        <v>17.896233588920659</v>
+      </c>
+      <c r="G11">
+        <v>5.4912996643327876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>